<commit_message>
Not the commit I want, but the commit I needed
</commit_message>
<xml_diff>
--- a/Opflix/Modelo_Fisico_Opflix.xlsx
+++ b/Opflix/Modelo_Fisico_Opflix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46885473820\Documents\Git\2s2019-sprint-bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46885473820\Documents\Git\2s2019-sprint-1-bd\Opflix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04A46BFC-5EAD-4964-A761-0A1D4AE10B59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD6F862-E4C2-4B1C-9CA1-33DBDC37E65A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955" xr2:uid="{80F540BC-CCCA-4671-8D49-1C1739F7645D}"/>
   </bookViews>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,13 +200,163 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF25FF92"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9DEBB0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98449E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF84D2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -250,27 +400,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -280,6 +493,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBF84D2"/>
+      <color rgb="FF98449E"/>
+      <color rgb="FF9DEBB0"/>
+      <color rgb="FF25FF92"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -590,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC73B448-D583-4688-BA84-904533F3DC06}">
   <dimension ref="B2:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,483 +830,483 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="K2" s="9"/>
+      <c r="M2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="K3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="7">
         <v>1111</v>
       </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="7">
         <v>2222</v>
       </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="11">
+        <v>2</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="2">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="M5" s="14">
+        <v>2</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E6" s="2">
+      <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="7">
         <v>3333</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="M6" s="2">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="M6" s="14">
         <v>3</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>4</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="7">
         <v>4444</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="15"/>
+      <c r="E10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="18"/>
+      <c r="H10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="5" t="s">
+      <c r="L11" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
+      <c r="H12" s="27">
+        <v>1</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="27">
         <v>3</v>
       </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="L12" s="27">
+        <v>1</v>
+      </c>
+      <c r="M12" s="27">
+        <v>1</v>
+      </c>
+      <c r="N12" s="27">
         <v>123</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="28">
         <v>43489</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="17">
+        <v>1</v>
+      </c>
+      <c r="C13" s="17">
         <v>5</v>
       </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="20">
+        <v>2</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="2">
-        <v>2</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="H13" s="27">
+        <v>2</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="2">
-        <v>2</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="K13" s="27">
+        <v>2</v>
+      </c>
+      <c r="L13" s="27">
+        <v>1</v>
+      </c>
+      <c r="M13" s="27">
+        <v>1</v>
+      </c>
+      <c r="N13" s="27">
         <v>108</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="28">
         <v>43669</v>
       </c>
-      <c r="P13" s="2"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
+      <c r="C14" s="17">
         <v>3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="20">
         <v>3</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="27">
         <v>3</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="K14" s="27">
+        <v>1</v>
+      </c>
+      <c r="L14" s="27">
+        <v>1</v>
+      </c>
+      <c r="M14" s="27">
+        <v>1</v>
+      </c>
+      <c r="N14" s="27">
         <v>117</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="28">
         <v>43589</v>
       </c>
-      <c r="P14" s="2"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="B15" s="17">
+        <v>2</v>
+      </c>
+      <c r="C15" s="17">
+        <v>2</v>
+      </c>
+      <c r="E15" s="20">
         <v>4</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="27">
         <v>4</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="27">
         <v>5</v>
       </c>
-      <c r="L15" s="2">
-        <v>2</v>
-      </c>
-      <c r="M15" s="2">
+      <c r="L15" s="27">
+        <v>2</v>
+      </c>
+      <c r="M15" s="27">
         <v>8</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="27">
         <v>496</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="28">
         <v>43632</v>
       </c>
-      <c r="P15" s="2"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="17">
+        <v>2</v>
+      </c>
+      <c r="C16" s="17">
         <v>4</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="20">
         <v>5</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="B17" s="17">
         <v>3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="17">
         <v>3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="17">
         <v>3</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="17">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="C19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="E21" s="23">
+        <v>1</v>
+      </c>
+      <c r="F21" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="2">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="23">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="2">
+      <c r="E23" s="23">
         <v>3</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="2">
+      <c r="E24" s="23">
         <v>4</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="23">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
+      <c r="E25" s="23">
         <v>4</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="23">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H10:P10"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H10:P10"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{5DE2974C-B6AA-4204-BE99-B5A2B2E7E397}"/>
@@ -1094,5 +1315,6 @@
     <hyperlink ref="G7" r:id="rId4" xr:uid="{A3C4C6BD-CC2D-4D4F-B90D-873F20CD2A9F}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>